<commit_message>
18 no fields added.
</commit_message>
<xml_diff>
--- a/Link Exchange Details - Flick.xlsx
+++ b/Link Exchange Details - Flick.xlsx
@@ -10473,7 +10473,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -11027,6 +11027,11 @@
         <v>9</v>
       </c>
     </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="10">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>